<commit_message>
fix sample time for sample 200207_0_6
</commit_message>
<xml_diff>
--- a/data/raw/design/20200129_design.xlsx
+++ b/data/raw/design/20200129_design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="strains" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,9 +96,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="HH:MM"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
-    <numFmt numFmtId="167" formatCode="MM/DD/YY\ HH:MM\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -192,12 +192,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -210,13 +210,10 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="D10:D13 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="A9 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.83"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -423,16 +420,15 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10:D13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="A9 D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,20 +721,18 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="D10:D13 A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,7 +849,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>44014.375</v>
+        <v>43984.375</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>

</xml_diff>